<commit_message>
Document updated by anvar
</commit_message>
<xml_diff>
--- a/Change Request and Requirements/WebsiteChanges.xlsx
+++ b/Change Request and Requirements/WebsiteChanges.xlsx
@@ -1,30 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hi\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8772"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="8775"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Activity</t>
   </si>
@@ -114,12 +104,27 @@
   </si>
   <si>
     <t>As of now we can remove the Blog screen as well</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>As of now hide Account button</t>
+  </si>
+  <si>
+    <t>Course Contents</t>
+  </si>
+  <si>
+    <t>Place the suitable image in the background with respect to courses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For Exmaple, If we choose AWS, then background image should be AWS </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -167,11 +172,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -184,9 +193,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -481,7 +487,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -489,22 +495,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -518,7 +524,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -532,7 +538,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -549,22 +555,22 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E4" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E5" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E6" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="D8" s="3" t="s">
         <v>12</v>
       </c>
@@ -572,17 +578,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E9" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E10" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3</v>
       </c>
@@ -593,7 +599,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>4</v>
       </c>
@@ -605,7 +611,7 @@
       </c>
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>5</v>
       </c>
@@ -617,7 +623,7 @@
       </c>
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>6</v>
       </c>
@@ -628,7 +634,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="43.15" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>7</v>
       </c>
@@ -642,7 +648,7 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>8</v>
       </c>
@@ -651,6 +657,34 @@
       </c>
       <c r="C17" s="4" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>9</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>10</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>